<commit_message>
RTL Updates:    -updated the control_unit_v2 to support AUIPC,LUI and JALR instructions    -did improvements over some small design components in cpu_pipeline_v2    -updated cpu_pipeline_v2 to support AUIPC,LUI and JALR instructions, also modified address compute logic for JAL    -updated cpu_sign_extend_unit to support U-Type instructions according to the RV32I spec Script Updates:    -updated assembler script to detect if a variable/label has been redefined and throw an error    -fixed bug when computing addresses of the variables for the symbol table
</commit_message>
<xml_diff>
--- a/RTL/Memory/MPU - Memory Map.xlsx
+++ b/RTL/Memory/MPU - Memory Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\Memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE72976-4401-4674-9889-E13AC1944B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D203B406-E7BA-4AC6-9DC0-93462D5457AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12945" yWindow="510" windowWidth="15765" windowHeight="14490" xr2:uid="{067881A5-A6BC-4587-B776-212172251E8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{067881A5-A6BC-4587-B776-212172251E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>0x00000000</t>
   </si>
   <si>
-    <t>0x0000FFFC</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
     <t>0xFFFFF800</t>
   </si>
   <si>
-    <t>0xFFFFFFFC</t>
-  </si>
-  <si>
-    <t>0xFFFFF7FC</t>
-  </si>
-  <si>
     <t>I/O
 Ports</t>
   </si>
@@ -208,13 +199,7 @@
 Address</t>
   </si>
   <si>
-    <t>0xFFFFEFFC</t>
-  </si>
-  <si>
     <t>0xFFFFF000</t>
-  </si>
-  <si>
-    <t>0x0FFFFFFC</t>
   </si>
   <si>
     <t>0x10000000</t>
@@ -224,9 +209,6 @@
 (~268MB)</t>
   </si>
   <si>
-    <t>0x10000FFC</t>
-  </si>
-  <si>
     <t>0x10001000</t>
   </si>
   <si>
@@ -234,9 +216,6 @@
 (~4KB)</t>
   </si>
   <si>
-    <t>0xBFFFFFFC</t>
-  </si>
-  <si>
     <t>0xC0000000</t>
   </si>
   <si>
@@ -263,6 +242,27 @@
   <si>
     <t>Future Expansion
 (~1GB)</t>
+  </si>
+  <si>
+    <t>0xFFFFFFFF</t>
+  </si>
+  <si>
+    <t>0xFFFFF7FF</t>
+  </si>
+  <si>
+    <t>0xFFFFEFFF</t>
+  </si>
+  <si>
+    <t>0xBFFFFFFF</t>
+  </si>
+  <si>
+    <t>0x10000FFF</t>
+  </si>
+  <si>
+    <t>0x0FFFFFFF</t>
+  </si>
+  <si>
+    <t>0x0000FFFF</t>
   </si>
 </sst>
 </file>
@@ -785,8 +785,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -797,12 +830,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -818,16 +845,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -835,24 +853,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1191,7 +1191,7 @@
   <dimension ref="B1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,63 +1210,63 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
       <c r="L2" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" s="42" t="s">
-        <v>54</v>
+        <v>29</v>
+      </c>
+      <c r="N2" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="39"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="43"/>
+        <v>28</v>
+      </c>
+      <c r="M3" s="25"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="36"/>
     </row>
     <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N4" s="9">
         <v>0</v>
@@ -1282,22 +1282,22 @@
     </row>
     <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="36"/>
+        <v>9</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="30"/>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H5">
         <f>(HEX2DEC(MID(B4,3,99))-HEX2DEC(MID(B6,3,99)))/4</f>
         <v>512</v>
       </c>
-      <c r="L5" s="44" t="s">
-        <v>33</v>
+      <c r="L5" s="31" t="s">
+        <v>30</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N5" s="21">
         <f>N4+1</f>
@@ -1314,20 +1314,20 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>13</v>
+        <v>66</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="45"/>
+        <v>17</v>
+      </c>
+      <c r="L6" s="32"/>
       <c r="M6" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N6" s="15">
         <f t="shared" ref="N6:N26" si="1">N5+1</f>
@@ -1337,24 +1337,24 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF808</v>
       </c>
-      <c r="P6" s="39"/>
+      <c r="P6" s="25"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="36"/>
+        <v>52</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="30"/>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7">
         <f>(HEX2DEC(MID(B6,3,99))-HEX2DEC(MID(B8,3,99)))/4</f>
         <v>512</v>
       </c>
-      <c r="L7" s="45"/>
+      <c r="L7" s="32"/>
       <c r="M7" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N7" s="15">
         <f t="shared" si="1"/>
@@ -1364,19 +1364,19 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF80C</v>
       </c>
-      <c r="P7" s="39"/>
+      <c r="P7" s="25"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="L8" s="46"/>
+        <v>67</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="L8" s="33"/>
       <c r="M8" s="19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N8" s="18">
         <f t="shared" si="1"/>
@@ -1386,19 +1386,19 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF810</v>
       </c>
-      <c r="P8" s="25"/>
+      <c r="P8" s="26"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="36"/>
-      <c r="L9" s="47" t="s">
-        <v>34</v>
+        <v>57</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="30"/>
+      <c r="L9" s="34" t="s">
+        <v>31</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N9" s="12">
         <f t="shared" si="1"/>
@@ -1415,17 +1415,17 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="32"/>
       <c r="M10" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N10" s="15">
         <f t="shared" si="1"/>
@@ -1435,17 +1435,17 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF818</v>
       </c>
-      <c r="P10" s="39"/>
+      <c r="P10" s="25"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="35"/>
-      <c r="L11" s="45"/>
+        <v>55</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="44"/>
+      <c r="L11" s="32"/>
       <c r="M11" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N11" s="15">
         <f t="shared" si="1"/>
@@ -1455,22 +1455,22 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF81C</v>
       </c>
-      <c r="P11" s="39"/>
+      <c r="P11" s="25"/>
     </row>
     <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="35"/>
+        <v>69</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="44"/>
       <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="46"/>
+        <v>12</v>
+      </c>
+      <c r="L12" s="33"/>
       <c r="M12" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N12" s="18">
         <f t="shared" si="1"/>
@@ -1480,26 +1480,26 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF820</v>
       </c>
-      <c r="P12" s="25"/>
+      <c r="P12" s="26"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="36"/>
+        <v>53</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="30"/>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H13">
         <f>(HEX2DEC(MID(B14,3,99))-HEX2DEC(MID(B16,3,99)))/4</f>
         <v>67092480</v>
       </c>
-      <c r="L13" s="47" t="s">
-        <v>49</v>
+      <c r="L13" s="34" t="s">
+        <v>46</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N13" s="12">
         <f t="shared" si="1"/>
@@ -1516,24 +1516,24 @@
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="43" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H14">
         <f>(HEX2DEC(MID(B15,3,99))-HEX2DEC(MID(B17,3,99)))/4</f>
         <v>16384</v>
       </c>
-      <c r="L14" s="45"/>
+      <c r="L14" s="32"/>
       <c r="M14" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N14" s="15">
         <f t="shared" si="1"/>
@@ -1543,17 +1543,17 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF828</v>
       </c>
-      <c r="P14" s="39"/>
+      <c r="P14" s="25"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="35"/>
-      <c r="L15" s="45"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="44"/>
+      <c r="L15" s="32"/>
       <c r="M15" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N15" s="15">
         <f t="shared" si="1"/>
@@ -1563,19 +1563,19 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF82C</v>
       </c>
-      <c r="P15" s="39"/>
+      <c r="P15" s="25"/>
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="35"/>
-      <c r="L16" s="46"/>
+        <v>71</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="L16" s="33"/>
       <c r="M16" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="1"/>
@@ -1585,19 +1585,19 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF830</v>
       </c>
-      <c r="P16" s="25"/>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="36"/>
-      <c r="L17" s="47" t="s">
-        <v>50</v>
+      <c r="C17" s="28"/>
+      <c r="D17" s="30"/>
+      <c r="L17" s="34" t="s">
+        <v>47</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="N17" s="12">
         <f t="shared" si="1"/>
@@ -1613,56 +1613,56 @@
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L18" s="45"/>
+      <c r="L18" s="32"/>
       <c r="M18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="O18" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF838</v>
+      </c>
+      <c r="P18" s="25"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L19" s="32"/>
+      <c r="M19" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="15">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="O19" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF83C</v>
+      </c>
+      <c r="P19" s="25"/>
+    </row>
+    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="33"/>
+      <c r="M20" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N20" s="18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="O20" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF840</v>
+      </c>
+      <c r="P20" s="26"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L21" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="N18" s="15">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="O18" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF838</v>
-      </c>
-      <c r="P18" s="39"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L19" s="45"/>
-      <c r="M19" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="N19" s="15">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="O19" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF83C</v>
-      </c>
-      <c r="P19" s="39"/>
-    </row>
-    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L20" s="46"/>
-      <c r="M20" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="N20" s="18">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="O20" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF840</v>
-      </c>
-      <c r="P20" s="25"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L21" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="M21" s="22" t="s">
-        <v>45</v>
       </c>
       <c r="N21" s="21">
         <f t="shared" si="1"/>
@@ -1678,9 +1678,9 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L22" s="45"/>
+      <c r="L22" s="32"/>
       <c r="M22" s="16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N22" s="15">
         <f t="shared" si="1"/>
@@ -1690,12 +1690,12 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF848</v>
       </c>
-      <c r="P22" s="39"/>
+      <c r="P22" s="25"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="45"/>
+      <c r="L23" s="32"/>
       <c r="M23" s="16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="1"/>
@@ -1705,12 +1705,12 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF84C</v>
       </c>
-      <c r="P23" s="39"/>
+      <c r="P23" s="25"/>
     </row>
     <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L24" s="46"/>
+      <c r="L24" s="33"/>
       <c r="M24" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N24" s="18">
         <f t="shared" si="1"/>
@@ -1720,14 +1720,14 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF850</v>
       </c>
-      <c r="P24" s="25"/>
+      <c r="P24" s="26"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="L25" s="24" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="N25" s="12">
         <f t="shared" si="1"/>
@@ -1743,9 +1743,9 @@
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L26" s="25"/>
+      <c r="L26" s="26"/>
       <c r="M26" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="N26" s="18">
         <f t="shared" si="1"/>
@@ -1755,23 +1755,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF858</v>
       </c>
-      <c r="P26" s="25"/>
+      <c r="P26" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P21:P24"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="L13:L16"/>
-    <mergeCell ref="L17:L20"/>
-    <mergeCell ref="L21:L24"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="P5:P8"/>
-    <mergeCell ref="P9:P12"/>
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="P17:P20"/>
     <mergeCell ref="L25:L26"/>
     <mergeCell ref="P25:P26"/>
     <mergeCell ref="B2:D2"/>
@@ -1788,6 +1775,19 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="P5:P8"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="P17:P20"/>
+    <mergeCell ref="P21:P24"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="L13:L16"/>
+    <mergeCell ref="L17:L20"/>
+    <mergeCell ref="L21:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>